<commit_message>
Update 2025-02-13 Artificial Lung Output.xlsx
</commit_message>
<xml_diff>
--- a/Data/2025-02-13 Artificial Lung Output.xlsx
+++ b/Data/2025-02-13 Artificial Lung Output.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Downloads\breath_easy\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EF7846-D0DA-42BA-B97E-4FC44A4D37E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8569423-43EE-4A51-818B-F7F39C0B8697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E3152FFF-FD09-4EEC-A97E-6D7D2308A030}"/>
   </bookViews>
@@ -36,12 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Output</t>
+    <t>ms</t>
   </si>
   <si>
-    <t>ms</t>
+    <t>Arduino Output</t>
+  </si>
+  <si>
+    <t>Artificial Lung</t>
   </si>
 </sst>
 </file>
@@ -111,6 +114,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Device</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Reading &amp; Artificial Lung Reading vs Time</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -155,7 +188,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Output</c:v>
+                  <c:v>Arduino Output</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -449,6 +482,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -511,6 +599,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Output (L/min)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1167,13 +1310,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1518,23 +1661,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85B730EF-6D66-4FCF-BBB9-8545DC3F4312}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1542,7 +1692,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1550,7 +1700,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1558,7 +1708,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1566,7 +1716,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1574,7 +1724,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1582,7 +1732,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1590,7 +1740,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1598,7 +1748,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1606,7 +1756,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1614,7 +1764,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1622,7 +1772,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1630,7 +1780,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1638,7 +1788,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1646,7 +1796,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>